<commit_message>
Add enhanced bulk match upload functionality for admins
Introduces a new admin page for uploading match data via Excel, including support for "league" match types and improved error handling.

Replit-Commit-Author: Agent
Replit-Commit-Session-Id: afbfe8a0-c5d4-4dfd-9b58-5f6304cce5ca
Replit-Commit-Checkpoint-Type: full_checkpoint
Replit-Commit-Screenshot-Url: https://storage.googleapis.com/screenshot-production-us-central1/7c53293f-df0f-44d1-aa13-74da41f82777/afbfe8a0-c5d4-4dfd-9b58-5f6304cce5ca/DX78Guq
</commit_message>
<xml_diff>
--- a/bulk-upload-test.xlsx
+++ b/bulk-upload-test.xlsx
@@ -407,7 +407,7 @@
         <v>Match Date (YYYY-MM-DD)</v>
       </c>
       <c r="B1" t="str">
-        <v>Match Type (casual/tournament)</v>
+        <v>Match Type (casual/tournament/league)</v>
       </c>
       <c r="C1" t="str">
         <v>Player 1 Passport Code</v>
@@ -569,37 +569,43 @@
       <c r="D3" t="str">
         <v>male</v>
       </c>
+      <c r="E3">
+        <v>31116</v>
+      </c>
       <c r="F3" t="str">
         <v>IPMDY2LM</v>
       </c>
       <c r="G3" t="str">
         <v>male</v>
       </c>
-      <c r="N3" t="b">
+      <c r="H3">
+        <v>33076</v>
+      </c>
+      <c r="O3" t="b">
         <v>0</v>
       </c>
-      <c r="O3">
+      <c r="P3">
         <v>2</v>
       </c>
-      <c r="P3">
+      <c r="Q3">
         <v>0</v>
       </c>
-      <c r="Q3">
-        <v>11</v>
-      </c>
       <c r="R3">
+        <v>11</v>
+      </c>
+      <c r="S3">
         <v>8</v>
       </c>
-      <c r="S3">
-        <v>11</v>
-      </c>
       <c r="T3">
+        <v>11</v>
+      </c>
+      <c r="U3">
         <v>6</v>
       </c>
-      <c r="W3" t="str">
+      <c r="X3" t="str">
         <v>Tournament Court A</v>
       </c>
-      <c r="X3" t="str">
+      <c r="Y3" t="str">
         <v>Singles tournament match - straight sets</v>
       </c>
     </row>
@@ -616,43 +622,49 @@
       <c r="D4" t="str">
         <v>male</v>
       </c>
+      <c r="E4">
+        <v>32452</v>
+      </c>
       <c r="F4" t="str">
         <v>WH67ZGSV</v>
       </c>
       <c r="G4" t="str">
         <v>female</v>
       </c>
-      <c r="N4" t="b">
+      <c r="H4">
+        <v>33865</v>
+      </c>
+      <c r="O4" t="b">
         <v>0</v>
       </c>
-      <c r="O4">
+      <c r="P4">
         <v>1</v>
       </c>
-      <c r="P4">
+      <c r="Q4">
         <v>2</v>
       </c>
-      <c r="Q4">
+      <c r="R4">
         <v>9</v>
       </c>
-      <c r="R4">
-        <v>11</v>
-      </c>
       <c r="S4">
+        <v>11</v>
+      </c>
+      <c r="T4">
         <v>10</v>
       </c>
-      <c r="T4">
+      <c r="U4">
         <v>12</v>
       </c>
-      <c r="U4">
-        <v>11</v>
-      </c>
       <c r="V4">
+        <v>11</v>
+      </c>
+      <c r="W4">
         <v>13</v>
       </c>
-      <c r="W4" t="str">
+      <c r="X4" t="str">
         <v>Court 2</v>
       </c>
-      <c r="X4" t="str">
+      <c r="Y4" t="str">
         <v>Close singles match with three games</v>
       </c>
     </row>
@@ -661,7 +673,7 @@
         <v>45883</v>
       </c>
       <c r="B5" t="str">
-        <v>casual</v>
+        <v>league</v>
       </c>
       <c r="C5" t="str">
         <v>LEE40BYN</v>
@@ -724,7 +736,7 @@
         <v>Court 3</v>
       </c>
       <c r="Y5" t="str">
-        <v>Doubles match - Team 2 wins in straight sets</v>
+        <v>League doubles match - Team 2 wins in straight sets</v>
       </c>
     </row>
     <row r="6">

</xml_diff>